<commit_message>
no desenho do banco de dados
</commit_message>
<xml_diff>
--- a/API/Métodos criados.xlsx
+++ b/API/Métodos criados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t xml:space="preserve">Método</t>
   </si>
@@ -31,7 +31,13 @@
     <t xml:space="preserve">Descrição</t>
   </si>
   <si>
-    <t xml:space="preserve">Get</t>
+    <t xml:space="preserve">Dados Esperados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dados Retornados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET</t>
   </si>
   <si>
     <t xml:space="preserve">/usuarios</t>
@@ -40,19 +46,37 @@
     <t xml:space="preserve">Rota para obter todos os usuários</t>
   </si>
   <si>
-    <t xml:space="preserve">Post</t>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lista de usuários (JSON)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para cadastrar um usuário</t>
   </si>
   <si>
+    <t xml:space="preserve">{ "nome": "string", "senha": "string", "cpf": "string", "email": "string" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Usuário cadastrado com sucesso!", "userId": number }</t>
+  </si>
+  <si>
     <t xml:space="preserve">/usuarios/login</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para consultar um usuário pelo CPF ou e-mail</t>
   </si>
   <si>
-    <t xml:space="preserve">Put</t>
+    <t xml:space="preserve">cpf: string OR email: string (pelo menos um deve ser fornecido)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuário encontrado (JSON)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT</t>
   </si>
   <si>
     <t xml:space="preserve">/usuarios/senha</t>
@@ -61,73 +85,154 @@
     <t xml:space="preserve">Rota para alterar a senha do usuário</t>
   </si>
   <si>
+    <t xml:space="preserve">{ "cpf": "string", "email": "string", "novaSenha": "string" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Senha alterada com sucesso!" }</t>
+  </si>
+  <si>
     <t xml:space="preserve">/copos</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para cadastrar um copo</t>
   </si>
   <si>
+    <t xml:space="preserve">{ "usuario_id": number, "nome": "string", "marca": "string", "capacidade_ml": number }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Copo cadastrado com sucesso!", "copoId": number }</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rota para obter todos os copos</t>
   </si>
   <si>
-    <t xml:space="preserve">/copos:id</t>
+    <t xml:space="preserve">Lista de copos (JSON)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/copos/:id</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para alterar os dados de um copo</t>
   </si>
   <si>
+    <t xml:space="preserve">{ "nome": "string", "marca": "string", "capacidade_ml": number }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Copo atualizado com sucesso!" }</t>
+  </si>
+  <si>
     <t xml:space="preserve">/copos/usuario/:usuario_id</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para consultar copos de um usuário específico</t>
   </si>
   <si>
+    <t xml:space="preserve">Lista de copos do usuário (JSON)</t>
+  </si>
+  <si>
     <t xml:space="preserve">/copos/ranking/:copo_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Rota para listar os 10 primeiros copos ordenados pela coluna k_med, incluindo um copo específico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/copos/:id</t>
+    <t xml:space="preserve">Rota para listar os 10 primeiros copos ordenados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lista de copos (JSON) incluindo o copo específico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para excluir um copo</t>
   </si>
   <si>
+    <t xml:space="preserve">{ "message": "Copo excluído com sucesso!" }</t>
+  </si>
+  <si>
     <t xml:space="preserve">/testes</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para obter todos os testes</t>
   </si>
   <si>
+    <t xml:space="preserve">Lista de testes (JSON)</t>
+  </si>
+  <si>
     <t xml:space="preserve">/teste/:id</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para obter um teste específico</t>
   </si>
   <si>
+    <t xml:space="preserve">id: number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detalhes do teste (JSON)</t>
+  </si>
+  <si>
     <t xml:space="preserve">/testes/copo/:copo_id</t>
   </si>
   <si>
     <t xml:space="preserve">Rota para obter todos os testes de um copo específico</t>
   </si>
   <si>
-    <t xml:space="preserve">/testes/:teste_id </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rota para excluir um teste específico de um copo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rota para acionar a API para novo teste, devendo ser informado usuário_id, tipo de teste e até 3 copo_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/resultadosTestes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rota para inserção dos dados do teste no Banco, acionadas por requisição do IoT à API na finalização do teste</t>
+    <t xml:space="preserve">copo_id: number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lista de testes do copo (JSON)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/testes/:teste_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rota para excluir um teste específico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teste_id: number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Teste excluído com sucesso!" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rota para acionar a API para novo teste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "usuario_id": number, "tipo": "string", "copos": [number, number, ...] }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Solicitação de teste registrada!" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/comando-pendente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rota usada pelo IoT para buscar o próximo comando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "iniciar": true/false, "comando": {...} }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/comando-consumido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rota para notificar que pegou um comando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "id": number }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "ok": true, "message": "Comando marcado como executado." }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/resultadosTestes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rota para registrar os resultados de um teste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "usuario_id": number, "copo_id": number, "tipo": "string", "data_inicio": "ISO8601", "data_fim": "ISO8601", "t0": number, "k": number }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "message": "Resultado de teste registrado com sucesso!", "teste_id": number }</t>
   </si>
 </sst>
 </file>
@@ -137,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,10 +266,18 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b val="true"/>
+      <sz val="21"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -176,12 +289,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -210,21 +330,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -416,204 +540,341 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.07421875" defaultRowHeight="37.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="102.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="54.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="54.45"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>22</v>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>6</v>
+        <v>54</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>35</v>
+        <v>60</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no README da API
</commit_message>
<xml_diff>
--- a/API/Métodos criados.xlsx
+++ b/API/Métodos criados.xlsx
@@ -281,12 +281,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -339,7 +345,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,6 +366,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -542,8 +608,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.07421875" defaultRowHeight="37.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -880,7 +946,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="66" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>